<commit_message>
feat: DOENST MATTER WHAT I DO (AHHH) WHAT I THINK I ABOUT IS YOU (AHH) EVEN WHEN IM WITH MY BOO (AHHH) ALL I THINK ABOUT IS YOU
</commit_message>
<xml_diff>
--- a/2.3.C-3-2.xlsx
+++ b/2.3.C-3-2.xlsx
@@ -5,55 +5,95 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IAmTheMage\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nsm44\Desktop\trabalhoPO\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{016AF50D-7342-4D33-B773-CAC310D593BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD99B8E-ED13-43E6-85AF-EF19091E5589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{BBB8149A-7663-4D44-831C-27357179E4D8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{BBB8149A-7663-4D44-831C-27357179E4D8}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1 (2)" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$20:$G$20</definedName>
+    <definedName name="solver_adj" localSheetId="1" hidden="1">Sheet1!$B$20:$G$20</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">'Sheet1 (2)'!$B$20:$G$20</definedName>
+    <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_eng" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_lhs1" localSheetId="0" hidden="1">Sheet1!$H$13:$H$14</definedName>
-    <definedName name="solver_lhs2" localSheetId="0" hidden="1">Sheet1!$H$15:$H$19</definedName>
-    <definedName name="solver_lhs3" localSheetId="0" hidden="1">Sheet1!$H$3:$H$6</definedName>
-    <definedName name="solver_lhs4" localSheetId="0" hidden="1">Sheet1!$H$7:$H$12</definedName>
+    <definedName name="solver_lhs1" localSheetId="1" hidden="1">Sheet1!$H$13:$H$14</definedName>
+    <definedName name="solver_lhs1" localSheetId="0" hidden="1">'Sheet1 (2)'!$H$13:$H$14</definedName>
+    <definedName name="solver_lhs2" localSheetId="1" hidden="1">Sheet1!$H$15:$H$19</definedName>
+    <definedName name="solver_lhs2" localSheetId="0" hidden="1">'Sheet1 (2)'!$H$15:$H$19</definedName>
+    <definedName name="solver_lhs3" localSheetId="1" hidden="1">Sheet1!$H$3:$H$6</definedName>
+    <definedName name="solver_lhs3" localSheetId="0" hidden="1">'Sheet1 (2)'!$H$3:$H$6</definedName>
+    <definedName name="solver_lhs4" localSheetId="1" hidden="1">Sheet1!$H$7:$H$12</definedName>
+    <definedName name="solver_lhs4" localSheetId="0" hidden="1">'Sheet1 (2)'!$H$7:$H$12</definedName>
+    <definedName name="solver_mip" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="1" hidden="1">30</definedName>
     <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="1" hidden="1">0.075</definedName>
     <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
-    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="1" hidden="1">4</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">4</definedName>
+    <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$K$19</definedName>
+    <definedName name="solver_opt" localSheetId="1" hidden="1">Sheet1!$K$19</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">'Sheet1 (2)'!$J$19</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rel3" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rel4" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_rel4" localSheetId="0" hidden="1">3</definedName>
-    <definedName name="solver_rhs1" localSheetId="0" hidden="1">Sheet1!$J$13:$J$14</definedName>
-    <definedName name="solver_rhs2" localSheetId="0" hidden="1">Sheet1!$J$15:$J$19</definedName>
-    <definedName name="solver_rhs3" localSheetId="0" hidden="1">Sheet1!$J$3:$J$6</definedName>
-    <definedName name="solver_rhs4" localSheetId="0" hidden="1">Sheet1!$J$7:$J$12</definedName>
-    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rhs1" localSheetId="1" hidden="1">Sheet1!$J$13:$J$14</definedName>
+    <definedName name="solver_rhs1" localSheetId="0" hidden="1">'Sheet1 (2)'!$J$13:$J$14</definedName>
+    <definedName name="solver_rhs2" localSheetId="1" hidden="1">Sheet1!$J$15:$J$19</definedName>
+    <definedName name="solver_rhs2" localSheetId="0" hidden="1">'Sheet1 (2)'!$K$15:$K$19</definedName>
+    <definedName name="solver_rhs3" localSheetId="1" hidden="1">Sheet1!$J$3:$J$6</definedName>
+    <definedName name="solver_rhs3" localSheetId="0" hidden="1">'Sheet1 (2)'!$J$3:$J$6</definedName>
+    <definedName name="solver_rhs4" localSheetId="1" hidden="1">Sheet1!$J$7:$J$12</definedName>
+    <definedName name="solver_rhs4" localSheetId="0" hidden="1">'Sheet1 (2)'!$J$7:$J$12</definedName>
+    <definedName name="solver_rlx" localSheetId="1" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="1" hidden="1">100</definedName>
     <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="1" hidden="1">3</definedName>
     <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -77,7 +117,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -99,7 +139,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="37">
   <si>
     <t>Constraints</t>
   </si>
@@ -183,23 +223,43 @@
   </si>
   <si>
     <t>Taxa de juros empréstimo</t>
+  </si>
+  <si>
+    <t>Sobra 1</t>
+  </si>
+  <si>
+    <t>Sobra 2</t>
+  </si>
+  <si>
+    <t>Sobra 3</t>
+  </si>
+  <si>
+    <t>Sobra 4</t>
+  </si>
+  <si>
+    <t>Sobra 5</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -213,6 +273,38 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="4" tint="0.39997558519241921"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -265,18 +357,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -290,7 +395,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -605,11 +710,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8879C365-3D1C-4715-923A-0CE1AF560A35}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9869FA2-B7C9-442B-B46C-1D975093C5DA}">
   <dimension ref="A1:O20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -617,35 +722,36 @@
     <col min="1" max="1" width="40" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="26.42578125" customWidth="1"/>
     <col min="15" max="15" width="27.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
+      <c r="D1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>19</v>
       </c>
       <c r="B2">
@@ -666,13 +772,13 @@
       <c r="G2">
         <v>1</v>
       </c>
-      <c r="H2" cm="1">
+      <c r="H2" s="6" cm="1">
         <f t="array" ref="H2:H19">MMULT(B2:G19,TRANSPOSE(B20:G20))</f>
-        <v>2.1956747648041808</v>
+        <v>2.6217000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B3">
@@ -693,7 +799,7 @@
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="6">
         <v>0</v>
       </c>
       <c r="I3" t="s">
@@ -710,7 +816,7 @@
       </c>
     </row>
     <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B4">
@@ -731,8 +837,8 @@
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="H4">
-        <v>0</v>
+      <c r="H4" s="6">
+        <v>0.91039999999999999</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
@@ -741,14 +847,14 @@
         <v>1</v>
       </c>
       <c r="N4">
-        <v>1.0173000000000001</v>
+        <v>1.02</v>
       </c>
       <c r="O4">
-        <v>1.0182</v>
+        <v>1.0249999999999999</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B5">
@@ -769,7 +875,7 @@
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="6">
         <v>1</v>
       </c>
       <c r="I5" t="s">
@@ -780,7 +886,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="4" t="s">
         <v>16</v>
       </c>
       <c r="B6">
@@ -801,8 +907,8 @@
       <c r="G6">
         <v>1</v>
       </c>
-      <c r="H6">
-        <v>0.52420588235294041</v>
+      <c r="H6" s="6">
+        <v>0</v>
       </c>
       <c r="I6" t="s">
         <v>7</v>
@@ -812,7 +918,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B7">
@@ -833,7 +939,7 @@
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
+      <c r="H7" s="6">
         <v>0</v>
       </c>
       <c r="I7" t="s">
@@ -844,7 +950,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B8">
@@ -865,8 +971,8 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>0</v>
+      <c r="H8" s="6">
+        <v>0.91039999999999999</v>
       </c>
       <c r="I8" t="s">
         <v>8</v>
@@ -876,7 +982,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B9">
@@ -897,7 +1003,7 @@
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="6">
         <v>1</v>
       </c>
       <c r="I9" t="s">
@@ -908,7 +1014,7 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="A10" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B10">
@@ -929,8 +1035,8 @@
       <c r="G10">
         <v>1</v>
       </c>
-      <c r="H10">
-        <v>0.52420588235294041</v>
+      <c r="H10" s="6">
+        <v>0</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
@@ -940,7 +1046,7 @@
       </c>
     </row>
     <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="A11" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B11">
@@ -961,8 +1067,8 @@
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>0.50720332367686083</v>
+      <c r="H11" s="6">
+        <v>0.71130000000000004</v>
       </c>
       <c r="I11" t="s">
         <v>8</v>
@@ -972,7 +1078,7 @@
       </c>
     </row>
     <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B12">
@@ -993,8 +1099,8 @@
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="H12">
-        <v>0.16426555877437976</v>
+      <c r="H12" s="6">
+        <v>0</v>
       </c>
       <c r="I12" t="s">
         <v>8</v>
@@ -1004,7 +1110,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="A13" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B13">
@@ -1025,8 +1131,8 @@
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <v>0.50720332367686083</v>
+      <c r="H13" s="6">
+        <v>0.71130000000000004</v>
       </c>
       <c r="I13" t="s">
         <v>7</v>
@@ -1036,7 +1142,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="4" t="s">
         <v>18</v>
       </c>
       <c r="B14">
@@ -1057,8 +1163,8 @@
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="H14">
-        <v>0.16426555877437976</v>
+      <c r="H14" s="6">
+        <v>0</v>
       </c>
       <c r="I14" t="s">
         <v>7</v>
@@ -1068,8 +1174,8 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
+      <c r="A15" s="4" t="s">
+        <v>28</v>
       </c>
       <c r="B15">
         <v>1</v>
@@ -1078,7 +1184,7 @@
         <v>3</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1089,24 +1195,24 @@
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="H15">
-        <v>1</v>
+      <c r="H15" s="6">
+        <v>0.71130000000000004</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="J15">
-        <f>1-K15</f>
-        <v>1</v>
+        <f>-(-1-D20*D2+H15)</f>
+        <v>0.28869999999999996</v>
       </c>
       <c r="K15">
-        <f>-(-1-D20*D2+H15)</f>
-        <v>0</v>
+        <f>1-J15</f>
+        <v>0.71130000000000004</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
+      <c r="A16" s="4" t="s">
+        <v>29</v>
       </c>
       <c r="B16">
         <v>3.1</v>
@@ -1126,24 +1232,24 @@
       <c r="G16">
         <v>0</v>
       </c>
-      <c r="H16">
-        <v>1.9829942003342178</v>
+      <c r="H16" s="6">
+        <v>2.2050300000000003</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="J16">
-        <f>1-K16</f>
-        <v>1.9829942003342178</v>
+        <f>1-(H16)+J15*N4-D20*D2*O4+E20*E2</f>
+        <v>-1.5600000000037806E-4</v>
       </c>
       <c r="K16">
-        <f>1-(H16)+K15*N4-D20*D2*O4+E20*E2</f>
-        <v>-0.9829942003342178</v>
+        <f>1-J16</f>
+        <v>1.0001560000000005</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>23</v>
+      <c r="A17" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B17">
         <v>1.5</v>
@@ -1163,24 +1269,24 @@
       <c r="G17">
         <v>0</v>
       </c>
-      <c r="H17">
-        <v>0.51440664735372155</v>
+      <c r="H17" s="6">
+        <v>1.0669500000000001</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="J17">
-        <f>1-K17</f>
-        <v>0.51440664735372144</v>
+        <f>1-H17+J16*N4-E20*E2*O4+F20*F2</f>
+        <v>-2.6912000000023362E-4</v>
       </c>
       <c r="K17">
-        <f>1-H17+K16*N4-E20*E2*O4+F20*F2</f>
-        <v>0.48559335264627856</v>
+        <f>1-J17</f>
+        <v>1.0002691200000002</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>24</v>
+      <c r="A18" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="B18">
         <v>-1.8</v>
@@ -1200,24 +1306,24 @@
       <c r="G18">
         <v>0</v>
       </c>
-      <c r="H18">
-        <v>-1.2086439884122331</v>
+      <c r="H18" s="6">
+        <v>-1.28034</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="J18">
-        <f>1-K18</f>
-        <v>-1.2086439884122329</v>
+        <f>1-H18+J17*N4-F20*F2*O4+G20*G2</f>
+        <v>1.2550654975999995</v>
       </c>
       <c r="K18">
-        <f>1-H18+K17*N4-F20*F2*O4+G20*G2</f>
-        <v>2.2086439884122329</v>
+        <f>1-J18</f>
+        <v>-0.25506549759999952</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>25</v>
+      <c r="A19" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="B19">
         <v>-5</v>
@@ -1237,44 +1343,730 @@
       <c r="G19">
         <v>0</v>
       </c>
-      <c r="H19">
-        <v>-2.9959601829525675</v>
+      <c r="H19" s="6">
+        <v>-3.5565000000000002</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J19" s="5">
-        <f>1+K18*N4-K19-G20*G2*O4</f>
-        <v>-2.9959601829525679</v>
-      </c>
-      <c r="K19" s="4">
-        <f>1-H19+K18*N4-G20*G2*O4</f>
-        <v>5.709067282952569</v>
+      <c r="J19" s="7">
+        <f>1-H19+J18*N4-G20*G2*O4</f>
+        <v>5.8366668075519996</v>
+      </c>
+      <c r="K19">
+        <f>1+J18*N4-J19-G20*G2*O4</f>
+        <v>-3.5564999999999998</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20">
-        <v>0.50720332367686083</v>
+        <v>0.71130000000000004</v>
       </c>
       <c r="C20">
-        <v>0.16426555877437976</v>
+        <v>0</v>
       </c>
       <c r="D20">
         <v>0</v>
       </c>
       <c r="E20">
-        <v>0</v>
+        <v>0.91039999999999999</v>
       </c>
       <c r="F20">
         <v>1</v>
       </c>
       <c r="G20">
-        <v>0.52420588235294041</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B2:G19">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8879C365-3D1C-4715-923A-0CE1AF560A35}">
+  <dimension ref="A1:O20"/>
+  <sheetViews>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15:K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="40" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="26.42578125" customWidth="1"/>
+    <col min="15" max="15" width="27.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6" cm="1">
+        <f t="array" ref="H2:H19">MMULT(B2:G19,TRANSPOSE(B20:G20))</f>
+        <v>2.1980565167243364</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3" s="6">
+        <v>0</v>
+      </c>
+      <c r="I3" t="s">
+        <v>7</v>
+      </c>
+      <c r="J3">
+        <v>1</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" s="6">
+        <v>0</v>
+      </c>
+      <c r="I4" t="s">
+        <v>7</v>
+      </c>
+      <c r="J4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>1.02</v>
+      </c>
+      <c r="O4">
+        <v>1.0249999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>7</v>
+      </c>
+      <c r="J5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6" s="6">
+        <v>0.52735294117647036</v>
+      </c>
+      <c r="I6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7" s="6">
+        <v>0</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="6">
+        <v>0</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9" s="6">
+        <v>1</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6">
+        <v>0.52735294117647036</v>
+      </c>
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11" s="6">
+        <v>0.50605536332179912</v>
+      </c>
+      <c r="I11" t="s">
+        <v>8</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12" s="6">
+        <v>0.16464821222606696</v>
+      </c>
+      <c r="I12" t="s">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13" s="6">
+        <v>0.50605536332179912</v>
+      </c>
+      <c r="I13" t="s">
+        <v>7</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14" s="6">
+        <v>0.16464821222606696</v>
+      </c>
+      <c r="I14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15" s="6">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J15">
+        <f>1-K15</f>
+        <v>1</v>
+      </c>
+      <c r="K15">
+        <f>-(-1-D20*D2+H15)</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16">
+        <v>3.1</v>
+      </c>
+      <c r="C16">
+        <v>2.5</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1.9803921568627447</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J16">
+        <f>1-K16</f>
+        <v>1.9803921568627447</v>
+      </c>
+      <c r="K16">
+        <f>1-(H16)+K15*N4-D20*D2*O4+E20*E2</f>
+        <v>-0.98039215686274472</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17">
+        <v>1.5</v>
+      </c>
+      <c r="C17">
+        <v>-1.5</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>0.51211072664359825</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J17">
+        <f>1-K17</f>
+        <v>0.51211072664359791</v>
+      </c>
+      <c r="K17">
+        <f>1-H17+K16*N4-E20*E2*O4+F20*F2</f>
+        <v>0.48788927335640209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B18">
+        <v>-1.8</v>
+      </c>
+      <c r="C18">
+        <v>-1.8</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18" s="6">
+        <v>-1.2072664359861589</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J18">
+        <f>1-K18</f>
+        <v>-1.2072664359861598</v>
+      </c>
+      <c r="K18">
+        <f>1-H18+K17*N4-F20*F2*O4+G20*G2</f>
+        <v>2.2072664359861598</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B19">
+        <v>-5</v>
+      </c>
+      <c r="C19">
+        <v>-2.8</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="6">
+        <v>-2.9912918108419833</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J19">
+        <f>1+K18*N4-K19-G20*G2*O4</f>
+        <v>-2.9912918108419828</v>
+      </c>
+      <c r="K19" s="7">
+        <f>1-H19+K18*N4-G20*G2*O4</f>
+        <v>5.7021668108419838</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20">
+        <v>0.50605536332179912</v>
+      </c>
+      <c r="C20">
+        <v>0.16464821222606696</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>1</v>
+      </c>
+      <c r="G20">
+        <v>0.52735294117647036</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="B2:G19">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>